<commit_message>
tested on updates to apparatus
</commit_message>
<xml_diff>
--- a/test/template_results/TPBO-0.75_CO2_27C_results.xlsx
+++ b/test/template_results/TPBO-0.75_CO2_27C_results.xlsx
@@ -668,10 +668,10 @@
         <v>52</v>
       </c>
       <c r="H2">
-        <v>90.46963744105656</v>
+        <v>92.36860169715462</v>
       </c>
       <c r="I2">
-        <v>4.678967430211545</v>
+        <v>1.819015083414506</v>
       </c>
       <c r="J2" t="s">
         <v>31</v>
@@ -700,10 +700,10 @@
         <v>32</v>
       </c>
       <c r="H3">
-        <v>5.622819601549301</v>
+        <v>5.368215497467331</v>
       </c>
       <c r="I3">
-        <v>0.7467836903242102</v>
+        <v>0.36648016077864065</v>
       </c>
       <c r="J3" t="s">
         <v>33</v>
@@ -732,10 +732,10 @@
         <v>34</v>
       </c>
       <c r="H4">
-        <v>16.1007086195629</v>
+        <v>15.381177201712239</v>
       </c>
       <c r="I4">
-        <v>1.3645930233591723</v>
+        <v>0.4761645837834983</v>
       </c>
       <c r="J4" t="s">
         <v>35</v>
@@ -946,10 +946,10 @@
         <v>0.0008266117111481498</v>
       </c>
       <c r="P12">
-        <v>53.052803144835174</v>
+        <v>52.87600173852176</v>
       </c>
       <c r="Q12">
-        <v>3.939498772635011</v>
+        <v>1.8498667314869128</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -996,10 +996,10 @@
         <v>0.002344800993961342</v>
       </c>
       <c r="P13">
-        <v>83.39746299446738</v>
+        <v>83.70692705335281</v>
       </c>
       <c r="Q13">
-        <v>4.312715803770232</v>
+        <v>1.8086625703807682</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1046,10 +1046,10 @@
         <v>0.0037992829160363355</v>
       </c>
       <c r="P14">
-        <v>97.23619253094368</v>
+        <v>97.54526414383393</v>
       </c>
       <c r="Q14">
-        <v>4.572667282237769</v>
+        <v>1.8245274789006884</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1096,10 +1096,10 @@
         <v>0.005540677245177677</v>
       </c>
       <c r="P15">
-        <v>109.18847872329391</v>
+        <v>109.3122802817562</v>
       </c>
       <c r="Q15">
-        <v>4.935141016794223</v>
+        <v>1.9117807281521277</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1146,10 +1146,10 @@
         <v>0.007333642301627097</v>
       </c>
       <c r="P16">
-        <v>119.37002567854324</v>
+        <v>119.23485564423626</v>
       </c>
       <c r="Q16">
-        <v>5.344230950498289</v>
+        <v>2.03215487278341</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1196,10 +1196,10 @@
         <v>0.009217434257071567</v>
       </c>
       <c r="P17">
-        <v>128.75269085089246</v>
+        <v>128.32498050774956</v>
       </c>
       <c r="Q17">
-        <v>5.79387116485911</v>
+        <v>2.173085158612707</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1246,10 +1246,10 @@
         <v>0.010910424426502266</v>
       </c>
       <c r="P18">
-        <v>136.22527493580702</v>
+        <v>135.53970164476718</v>
       </c>
       <c r="Q18">
-        <v>6.194710548425781</v>
+        <v>2.3021739961767254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed volume defaults and removed transients from gas sorption template
</commit_message>
<xml_diff>
--- a/test/template_results/TPBO-0.75_CO2_27C_results.xlsx
+++ b/test/template_results/TPBO-0.75_CO2_27C_results.xlsx
@@ -668,10 +668,10 @@
         <v>52</v>
       </c>
       <c r="H2">
-        <v>92.36860169715462</v>
+        <v>92.3686016981486</v>
       </c>
       <c r="I2">
-        <v>1.819015083414506</v>
+        <v>1.819015081414576</v>
       </c>
       <c r="J2" t="s">
         <v>31</v>
@@ -700,10 +700,10 @@
         <v>32</v>
       </c>
       <c r="H3">
-        <v>5.368215497467331</v>
+        <v>5.368215497335185</v>
       </c>
       <c r="I3">
-        <v>0.36648016077864065</v>
+        <v>0.36648016046579185</v>
       </c>
       <c r="J3" t="s">
         <v>33</v>
@@ -732,10 +732,10 @@
         <v>34</v>
       </c>
       <c r="H4">
-        <v>15.381177201712239</v>
+        <v>15.38117720140261</v>
       </c>
       <c r="I4">
-        <v>0.4761645837834983</v>
+        <v>0.4761645833255455</v>
       </c>
       <c r="J4" t="s">
         <v>35</v>
@@ -946,10 +946,10 @@
         <v>0.0008266117111481498</v>
       </c>
       <c r="P12">
-        <v>52.87600173852176</v>
+        <v>52.87600173842287</v>
       </c>
       <c r="Q12">
-        <v>1.8498667314869128</v>
+        <v>1.8498667298241975</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -996,10 +996,10 @@
         <v>0.002344800993961342</v>
       </c>
       <c r="P13">
-        <v>83.70692705335281</v>
+        <v>83.70692705354358</v>
       </c>
       <c r="Q13">
-        <v>1.8086625703807682</v>
+        <v>1.8086625685739806</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1046,10 +1046,10 @@
         <v>0.0037992829160363355</v>
       </c>
       <c r="P14">
-        <v>97.54526414383393</v>
+        <v>97.54526414405993</v>
       </c>
       <c r="Q14">
-        <v>1.8245274789006884</v>
+        <v>1.8245274770055506</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1096,10 +1096,10 @@
         <v>0.005540677245177677</v>
       </c>
       <c r="P15">
-        <v>109.3122802817562</v>
+        <v>109.31228028192395</v>
       </c>
       <c r="Q15">
-        <v>1.9117807281521277</v>
+        <v>1.9117807261436952</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1146,10 +1146,10 @@
         <v>0.007333642301627097</v>
       </c>
       <c r="P16">
-        <v>119.23485564423626</v>
+        <v>119.23485564430503</v>
       </c>
       <c r="Q16">
-        <v>2.03215487278341</v>
+        <v>2.032154870652259</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1196,10 +1196,10 @@
         <v>0.009217434257071567</v>
       </c>
       <c r="P17">
-        <v>128.32498050774956</v>
+        <v>128.32498050770067</v>
       </c>
       <c r="Q17">
-        <v>2.173085158612707</v>
+        <v>2.173085156348046</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1246,10 +1246,10 @@
         <v>0.010910424426502266</v>
       </c>
       <c r="P18">
-        <v>135.53970164476718</v>
+        <v>135.5397016446123</v>
       </c>
       <c r="Q18">
-        <v>2.3021739961767254</v>
+        <v>2.302173993792711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
molar vol included in gsa now
</commit_message>
<xml_diff>
--- a/test/template_results/TPBO-0.75_CO2_27C_results.xlsx
+++ b/test/template_results/TPBO-0.75_CO2_27C_results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
   <si>
     <t>Overall Properties</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Dual Mode (CH')</t>
+  </si>
+  <si>
+    <t>Molar Vol (L/mol)</t>
+  </si>
+  <si>
+    <t>M. Vol. err (L/mol)</t>
   </si>
   <si>
     <t>Variable</t>
@@ -605,7 +611,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -613,7 +619,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -645,7 +651,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -677,7 +683,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -709,7 +715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -741,7 +747,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -761,7 +767,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -781,7 +787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -801,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -821,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -841,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -852,7 +858,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -890,19 +896,25 @@
         <v>43</v>
       </c>
       <c r="N11" t="s">
+        <v>53</v>
+      </c>
+      <c r="O11" t="s">
+        <v>54</v>
+      </c>
+      <c r="P11" t="s">
         <v>44</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>45</v>
       </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
         <v>46</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>1</v>
       </c>
@@ -940,19 +952,25 @@
         <v>0.00010534522772145979</v>
       </c>
       <c r="N12">
+        <v>11.437863057602693</v>
+      </c>
+      <c r="O12">
+        <v>0.005789915463944882</v>
+      </c>
+      <c r="P12">
         <v>0.0718661980992095</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>0.0008266117111481498</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>52.87600173842287</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>1.8498667298241975</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>2</v>
       </c>
@@ -990,19 +1008,25 @@
         <v>0.0003239596849754356</v>
       </c>
       <c r="N13">
+        <v>3.430803399487487</v>
+      </c>
+      <c r="O13">
+        <v>0.0017860378557054417</v>
+      </c>
+      <c r="P13">
         <v>0.10783827493962246</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>0.002344800993961342</v>
       </c>
-      <c r="P13">
+      <c r="R13">
         <v>83.70692705354358</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>1.8086625685739806</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1040,19 +1064,25 @@
         <v>0.0005113349942957766</v>
       </c>
       <c r="N14">
+        <v>2.0046748445944713</v>
+      </c>
+      <c r="O14">
+        <v>0.0010746059098845988</v>
+      </c>
+      <c r="P14">
         <v>0.12552168523371413</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>0.0037992829160363355</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>97.54526414405993</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>1.8245274770055506</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1090,19 +1120,25 @@
         <v>0.000698928298436255</v>
       </c>
       <c r="N15">
+        <v>1.3310716164493712</v>
+      </c>
+      <c r="O15">
+        <v>0.0007402721728057062</v>
+      </c>
+      <c r="P15">
         <v>0.13770619457731811</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>0.005540677245177677</v>
       </c>
-      <c r="P15">
+      <c r="R15">
         <v>109.31228028192395</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>1.9117807261436952</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1140,19 +1176,25 @@
         <v>0.0008550130872841051</v>
       </c>
       <c r="N16">
+        <v>0.9847644037805116</v>
+      </c>
+      <c r="O16">
+        <v>0.0005700445884418672</v>
+      </c>
+      <c r="P16">
         <v>0.14787002282207362</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>0.007333642301627097</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <v>119.23485564430503</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>2.032154870652259</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1190,19 +1232,25 @@
         <v>0.0009837338596060576</v>
       </c>
       <c r="N17">
+        <v>0.7710205285078638</v>
+      </c>
+      <c r="O17">
+        <v>0.0004666441566139297</v>
+      </c>
+      <c r="P17">
         <v>0.15739145672692484</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>0.009217434257071567</v>
       </c>
-      <c r="P17">
+      <c r="R17">
         <v>128.32498050770067</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>2.173085156348046</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1240,15 +1288,21 @@
         <v>0.0010714842747861742</v>
       </c>
       <c r="N18">
+        <v>0.6458420268502967</v>
+      </c>
+      <c r="O18">
+        <v>0.00040748136774608885</v>
+      </c>
+      <c r="P18">
         <v>0.16529358011808337</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>0.010910424426502266</v>
       </c>
-      <c r="P18">
+      <c r="R18">
         <v>135.5397016446123</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <v>2.302173993792711</v>
       </c>
     </row>
@@ -1267,52 +1321,52 @@
   <sheetData>
     <row r="2" spans="1:21">
       <c r="F2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="Q2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="R2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="S2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="T2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="U2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1356,13 +1410,13 @@
         <v>2.71</v>
       </c>
       <c r="S3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="T3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="U3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1406,13 +1460,13 @@
         <v>0.0</v>
       </c>
       <c r="S4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="T4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="U4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1420,37 +1474,37 @@
         <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" t="s">
         <v>59</v>
       </c>
-      <c r="K5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R5" t="s">
         <v>63</v>
-      </c>
-      <c r="M5" t="s">
-        <v>57</v>
-      </c>
-      <c r="N5" t="s">
-        <v>66</v>
-      </c>
-      <c r="O5" t="s">
-        <v>66</v>
-      </c>
-      <c r="P5" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>63</v>
-      </c>
-      <c r="R5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:21">

</xml_diff>

<commit_message>
more efficient loading new version
</commit_message>
<xml_diff>
--- a/test/template_results/TPBO-0.75_CO2_27C_results.xlsx
+++ b/test/template_results/TPBO-0.75_CO2_27C_results.xlsx
@@ -958,10 +958,10 @@
         <v>0.005789915463944882</v>
       </c>
       <c r="P12">
-        <v>0.0718661980992095</v>
+        <v>0.0375898586132879</v>
       </c>
       <c r="Q12">
-        <v>0.0008266117111481498</v>
+        <v>0.0005889352803773407</v>
       </c>
       <c r="R12">
         <v>52.87600173842287</v>
@@ -1014,10 +1014,10 @@
         <v>0.0017860378557054417</v>
       </c>
       <c r="P13">
-        <v>0.10783827493962246</v>
+        <v>0.05867943939644259</v>
       </c>
       <c r="Q13">
-        <v>0.002344800993961342</v>
+        <v>0.0005068691481518938</v>
       </c>
       <c r="R13">
         <v>83.70692705354358</v>
@@ -1070,10 +1070,10 @@
         <v>0.0010746059098845988</v>
       </c>
       <c r="P14">
-        <v>0.12552168523371413</v>
+        <v>0.06968291800307592</v>
       </c>
       <c r="Q14">
-        <v>0.0037992829160363355</v>
+        <v>0.0008593573285447139</v>
       </c>
       <c r="R14">
         <v>97.54526414405993</v>
@@ -1126,10 +1126,10 @@
         <v>0.0007402721728057062</v>
       </c>
       <c r="P15">
-        <v>0.13770619457731811</v>
+        <v>0.07752732911814221</v>
       </c>
       <c r="Q15">
-        <v>0.005540677245177677</v>
+        <v>0.0017373645222090906</v>
       </c>
       <c r="R15">
         <v>109.31228028192395</v>
@@ -1182,10 +1182,10 @@
         <v>0.0005700445884418672</v>
       </c>
       <c r="P16">
-        <v>0.14787002282207362</v>
+        <v>0.08424243429322628</v>
       </c>
       <c r="Q16">
-        <v>0.007333642301627097</v>
+        <v>0.0027979286560536696</v>
       </c>
       <c r="R16">
         <v>119.23485564430503</v>
@@ -1238,10 +1238,10 @@
         <v>0.0004666441566139297</v>
       </c>
       <c r="P17">
-        <v>0.15739145672692484</v>
+        <v>0.09068008289072088</v>
       </c>
       <c r="Q17">
-        <v>0.009217434257071567</v>
+        <v>0.004013519039213339</v>
       </c>
       <c r="R17">
         <v>128.32498050770067</v>
@@ -1294,10 +1294,10 @@
         <v>0.00040748136774608885</v>
       </c>
       <c r="P18">
-        <v>0.16529358011808337</v>
+        <v>0.09613440530926486</v>
       </c>
       <c r="Q18">
-        <v>0.010910424426502266</v>
+        <v>0.005198235451499367</v>
       </c>
       <c r="R18">
         <v>135.5397016446123</v>

</xml_diff>